<commit_message>
End of section 7
</commit_message>
<xml_diff>
--- a/General info Skinet project.xlsx
+++ b/General info Skinet project.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="CMD commands" sheetId="1" r:id="rId1"/>
     <sheet name="Visual code commands" sheetId="2" r:id="rId2"/>
     <sheet name="Section 5 - Error Heandling" sheetId="3" r:id="rId3"/>
+    <sheet name="Generics&amp;Specifications" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="86">
   <si>
     <t>command description</t>
   </si>
@@ -229,6 +230,84 @@
   </si>
   <si>
     <t>For flating the validation errors to a string array</t>
+  </si>
+  <si>
+    <t>File structure</t>
+  </si>
+  <si>
+    <t>Folder</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>IGenericRepository</t>
+  </si>
+  <si>
+    <t>Interfaces</t>
+  </si>
+  <si>
+    <t>Core</t>
+  </si>
+  <si>
+    <t>GenericRepository</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Infrastructure</t>
+  </si>
+  <si>
+    <t>SpecificationEvaluator</t>
+  </si>
+  <si>
+    <t>BaseSpecification</t>
+  </si>
+  <si>
+    <t>Ispecification</t>
+  </si>
+  <si>
+    <t>Specifications</t>
+  </si>
+  <si>
+    <t>ProductSpecParams</t>
+  </si>
+  <si>
+    <t>ProductsWithTypesAndBrandsSpecification</t>
+  </si>
+  <si>
+    <t>ProductWithFiltersForCountSpesifications</t>
+  </si>
+  <si>
+    <t>Pagination</t>
+  </si>
+  <si>
+    <t>Helpers</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>controller</t>
+  </si>
+  <si>
+    <t>ProductController</t>
+  </si>
+  <si>
+    <t>Controllers</t>
+  </si>
+  <si>
+    <t>spec</t>
+  </si>
+  <si>
+    <t>countspec</t>
+  </si>
+  <si>
+    <t>&lt;</t>
+  </si>
+  <si>
+    <t>=</t>
   </si>
 </sst>
 </file>
@@ -299,11 +378,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -808,7 +887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -822,11 +901,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2"/>
@@ -953,4 +1032,188 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="50.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="40.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" t="s">
+        <v>82</v>
+      </c>
+      <c r="I8" t="s">
+        <v>85</v>
+      </c>
+      <c r="J8" t="s">
+        <v>74</v>
+      </c>
+      <c r="K8" t="s">
+        <v>84</v>
+      </c>
+      <c r="M8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" t="s">
+        <v>83</v>
+      </c>
+      <c r="I10" t="s">
+        <v>85</v>
+      </c>
+      <c r="J10" t="s">
+        <v>75</v>
+      </c>
+      <c r="K10" t="s">
+        <v>84</v>
+      </c>
+      <c r="M10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
End of section 15
</commit_message>
<xml_diff>
--- a/General info Skinet project.xlsx
+++ b/General info Skinet project.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="CMD commands" sheetId="1" r:id="rId1"/>
     <sheet name="Visual code commands" sheetId="2" r:id="rId2"/>
     <sheet name="Section 5 - Error Heandling" sheetId="3" r:id="rId3"/>
     <sheet name="Generics&amp;Specifications" sheetId="4" r:id="rId4"/>
+    <sheet name="API - Identity" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="131">
   <si>
     <t>command description</t>
   </si>
@@ -308,6 +309,141 @@
   </si>
   <si>
     <t>=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Packages From Nuget Gallery </t>
+  </si>
+  <si>
+    <t>Packages Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Microsoft.AspNetCore.Identity.EntityFramworkCore</t>
+  </si>
+  <si>
+    <t>Contains all the Entity cores</t>
+  </si>
+  <si>
+    <t>Microsoft.AspNetCore.Identity</t>
+  </si>
+  <si>
+    <t>Contain the user_manger and SignIn_manager</t>
+  </si>
+  <si>
+    <t>Microsoft.IdentityModel.Tokens</t>
+  </si>
+  <si>
+    <t>Provide the support of security token</t>
+  </si>
+  <si>
+    <t>System.IdentityModel.Tokens.Jwt</t>
+  </si>
+  <si>
+    <t>Help us to create serialize and validate the Json web token</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Setting up the Identity classes</t>
+  </si>
+  <si>
+    <t>Create class AppUser and drive from class Identity</t>
+  </si>
+  <si>
+    <t>Add Identity to DbContext</t>
+  </si>
+  <si>
+    <t>Replaced the driven class with IdentityDbContext&lt;AppUser&gt;</t>
+  </si>
+  <si>
+    <t>Add a new Migration</t>
+  </si>
+  <si>
+    <t>This action will create all the entities related to the identity calss</t>
+  </si>
+  <si>
+    <t>Add DTOs</t>
+  </si>
+  <si>
+    <t>Add UserDto, LoginDto, RegisterDto</t>
+  </si>
+  <si>
+    <t>Adding register function to the AccountController</t>
+  </si>
+  <si>
+    <t>Adding login function to the AccountController</t>
+  </si>
+  <si>
+    <t>With [HttpPost("login")] create Async</t>
+  </si>
+  <si>
+    <t>With [HttpPost("register")] create Async</t>
+  </si>
+  <si>
+    <t>Create a new Interface ITokenService</t>
+  </si>
+  <si>
+    <t>string CreateToken(AppUser)</t>
+  </si>
+  <si>
+    <t>Add to autoMapper a new map</t>
+  </si>
+  <si>
+    <t>CreateMap&lt;Address, AddressDto&gt;().ReverseMap();</t>
+  </si>
+  <si>
+    <t>Create a new class call TokenService and drive from ITokenService</t>
+  </si>
+  <si>
+    <t>This service will be responsible for create and return token</t>
+  </si>
+  <si>
+    <t>Create IdentityServiceExtension</t>
+  </si>
+  <si>
+    <t>Configure authentication service and how it needs to validate</t>
+  </si>
+  <si>
+    <t>Configure authentication service on IdentityServiceExtension class</t>
+  </si>
+  <si>
+    <t>Add secret key and Issuer to appSetting.json</t>
+  </si>
+  <si>
+    <t>Set all Identity services in this file extension</t>
+  </si>
+  <si>
+    <t>Add IdentityServiceExtension to our startup class</t>
+  </si>
+  <si>
+    <t>services.AddIdentityServices(_config);</t>
+  </si>
+  <si>
+    <t>Add appAuthentication to our startup class</t>
+  </si>
+  <si>
+    <t>app.UseAuthentication();  need to be before app.UseAuthorization();</t>
+  </si>
+  <si>
+    <t>AddScoped service for tokenService</t>
+  </si>
+  <si>
+    <t>services.AddScoped&lt;ITokenService,TokenService&gt;();</t>
+  </si>
+  <si>
+    <t>Add Account controller</t>
+  </si>
+  <si>
+    <t>Inject UserManager&lt;AppUser&gt; userManager, SignInManager&lt;AppUser&gt; signInManager, ITokenService tokenService, IMapper mapper</t>
+  </si>
+  <si>
+    <t>Adding user manager extension methods</t>
+  </si>
+  <si>
+    <t>To return current user according the claims</t>
   </si>
 </sst>
 </file>
@@ -389,7 +525,14 @@
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -400,6 +543,30 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:C7" totalsRowShown="0">
+  <autoFilter ref="A3:C7"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="#" dataDxfId="1"/>
+    <tableColumn id="3" name="Packages Name"/>
+    <tableColumn id="2" name="Description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A12:C30" totalsRowShown="0">
+  <autoFilter ref="A12:C30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="#" dataDxfId="0"/>
+    <tableColumn id="2" name="Step"/>
+    <tableColumn id="3" name="Description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1038,8 +1205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1216,4 +1383,294 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C30"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="61.7109375" customWidth="1"/>
+    <col min="3" max="3" width="121.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>116</v>
+      </c>
+      <c r="C16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>121</v>
+      </c>
+      <c r="C18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>11</v>
+      </c>
+      <c r="B21" t="s">
+        <v>110</v>
+      </c>
+      <c r="C21" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>12</v>
+      </c>
+      <c r="B22" t="s">
+        <v>114</v>
+      </c>
+      <c r="C22" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>13</v>
+      </c>
+      <c r="B23" t="s">
+        <v>125</v>
+      </c>
+      <c r="C23" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>14</v>
+      </c>
+      <c r="B24" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>15</v>
+      </c>
+      <c r="B25" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>16</v>
+      </c>
+      <c r="B26" t="s">
+        <v>112</v>
+      </c>
+      <c r="C26" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>17</v>
+      </c>
+      <c r="B27" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>18</v>
+      </c>
+      <c r="B28" t="s">
+        <v>106</v>
+      </c>
+      <c r="C28" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>19</v>
+      </c>
+      <c r="B29" t="s">
+        <v>129</v>
+      </c>
+      <c r="C29" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>